<commit_message>
balance ingresos uci, al 18 de agosto 2021
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_ingresos.xlsx
+++ b/input/Camas_uci/last_ingresos.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilianocordova\Documents\03 SRA\99 Coronavirus\Corona\Reporte diario COVID-19\Reporte 210729\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauriciodiaz\Desktop\REPORTE DE CAMAS\MINISTERIO CIENCIAS\MEDIA MOVIL INGRESOS UCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACE5031-54DE-4BAD-8A98-71080805A38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -104,13 +114,13 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -391,21 +401,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:RE2"/>
+  <dimension ref="A1:RZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="RQ1" workbookViewId="0">
+      <selection activeCell="RZ2" sqref="RT2:RZ2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="30.08203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:473" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:494" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1582,1669 +1594,1795 @@
       <c r="OB1" s="1">
         <v>44318</v>
       </c>
-      <c r="OC1" s="2">
+      <c r="OC1" s="1">
         <v>44319</v>
       </c>
-      <c r="OD1" s="2">
+      <c r="OD1" s="1">
         <v>44320</v>
       </c>
-      <c r="OE1" s="2">
+      <c r="OE1" s="1">
         <v>44321</v>
       </c>
-      <c r="OF1" s="2">
+      <c r="OF1" s="1">
         <v>44322</v>
       </c>
-      <c r="OG1" s="2">
+      <c r="OG1" s="1">
         <v>44323</v>
       </c>
-      <c r="OH1" s="2">
+      <c r="OH1" s="1">
         <v>44324</v>
       </c>
-      <c r="OI1" s="2">
+      <c r="OI1" s="1">
         <v>44325</v>
       </c>
-      <c r="OJ1" s="2">
+      <c r="OJ1" s="1">
         <v>44326</v>
       </c>
-      <c r="OK1" s="2">
+      <c r="OK1" s="1">
         <v>44327</v>
       </c>
-      <c r="OL1" s="2">
+      <c r="OL1" s="1">
         <v>44328</v>
       </c>
-      <c r="OM1" s="2">
+      <c r="OM1" s="1">
         <v>44329</v>
       </c>
-      <c r="ON1" s="2">
+      <c r="ON1" s="1">
         <v>44330</v>
       </c>
-      <c r="OO1" s="2">
+      <c r="OO1" s="1">
         <v>44331</v>
       </c>
-      <c r="OP1" s="2">
+      <c r="OP1" s="1">
         <v>44332</v>
       </c>
-      <c r="OQ1" s="2">
+      <c r="OQ1" s="1">
         <v>44333</v>
       </c>
-      <c r="OR1" s="2">
+      <c r="OR1" s="1">
         <v>44334</v>
       </c>
-      <c r="OS1" s="2">
+      <c r="OS1" s="1">
         <v>44335</v>
       </c>
-      <c r="OT1" s="2">
+      <c r="OT1" s="1">
         <v>44336</v>
       </c>
-      <c r="OU1" s="2">
+      <c r="OU1" s="1">
         <v>44337</v>
       </c>
-      <c r="OV1" s="2">
+      <c r="OV1" s="1">
         <v>44338</v>
       </c>
-      <c r="OW1" s="2">
+      <c r="OW1" s="1">
         <v>44339</v>
       </c>
-      <c r="OX1" s="2">
+      <c r="OX1" s="1">
         <v>44340</v>
       </c>
-      <c r="OY1" s="2">
+      <c r="OY1" s="1">
         <v>44341</v>
       </c>
-      <c r="OZ1" s="2">
+      <c r="OZ1" s="1">
         <v>44342</v>
       </c>
-      <c r="PA1" s="2">
+      <c r="PA1" s="1">
         <v>44343</v>
       </c>
-      <c r="PB1" s="2">
+      <c r="PB1" s="1">
         <v>44344</v>
       </c>
-      <c r="PC1" s="2">
+      <c r="PC1" s="1">
         <v>44345</v>
       </c>
-      <c r="PD1" s="2">
+      <c r="PD1" s="1">
         <v>44346</v>
       </c>
-      <c r="PE1" s="2">
+      <c r="PE1" s="1">
         <v>44347</v>
       </c>
-      <c r="PF1" s="2">
+      <c r="PF1" s="1">
         <v>44348</v>
       </c>
-      <c r="PG1" s="2">
+      <c r="PG1" s="1">
         <v>44349</v>
       </c>
-      <c r="PH1" s="2">
+      <c r="PH1" s="1">
         <v>44350</v>
       </c>
-      <c r="PI1" s="2">
+      <c r="PI1" s="1">
         <v>44351</v>
       </c>
-      <c r="PJ1" s="2">
+      <c r="PJ1" s="1">
         <v>44352</v>
       </c>
-      <c r="PK1" s="2">
+      <c r="PK1" s="1">
         <v>44353</v>
       </c>
-      <c r="PL1" s="2">
+      <c r="PL1" s="1">
         <v>44354</v>
       </c>
-      <c r="PM1" s="2">
+      <c r="PM1" s="1">
         <v>44355</v>
       </c>
-      <c r="PN1" s="2">
+      <c r="PN1" s="1">
         <v>44356</v>
       </c>
-      <c r="PO1" s="2">
+      <c r="PO1" s="1">
         <v>44357</v>
       </c>
-      <c r="PP1" s="2">
+      <c r="PP1" s="1">
         <v>44358</v>
       </c>
-      <c r="PQ1" s="2">
+      <c r="PQ1" s="1">
         <v>44359</v>
       </c>
-      <c r="PR1" s="2">
+      <c r="PR1" s="1">
         <v>44360</v>
       </c>
-      <c r="PS1" s="2">
+      <c r="PS1" s="1">
         <v>44361</v>
       </c>
-      <c r="PT1" s="2">
+      <c r="PT1" s="1">
         <v>44362</v>
       </c>
-      <c r="PU1" s="2">
+      <c r="PU1" s="1">
         <v>44363</v>
       </c>
-      <c r="PV1" s="2">
+      <c r="PV1" s="1">
         <v>44364</v>
       </c>
-      <c r="PW1" s="2">
+      <c r="PW1" s="1">
         <v>44365</v>
       </c>
-      <c r="PX1" s="2">
+      <c r="PX1" s="1">
         <v>44366</v>
       </c>
-      <c r="PY1" s="2">
+      <c r="PY1" s="1">
         <v>44367</v>
       </c>
-      <c r="PZ1" s="2">
+      <c r="PZ1" s="1">
         <v>44368</v>
       </c>
-      <c r="QA1" s="2">
+      <c r="QA1" s="1">
         <v>44369</v>
       </c>
-      <c r="QB1" s="2">
+      <c r="QB1" s="1">
         <v>44370</v>
       </c>
-      <c r="QC1" s="2">
+      <c r="QC1" s="1">
         <v>44371</v>
       </c>
-      <c r="QD1" s="2">
+      <c r="QD1" s="1">
         <v>44372</v>
       </c>
-      <c r="QE1" s="2">
+      <c r="QE1" s="1">
         <v>44373</v>
       </c>
-      <c r="QF1" s="2">
+      <c r="QF1" s="1">
         <v>44374</v>
       </c>
-      <c r="QG1" s="2">
+      <c r="QG1" s="1">
         <v>44375</v>
       </c>
-      <c r="QH1" s="2">
+      <c r="QH1" s="1">
         <v>44376</v>
       </c>
-      <c r="QI1" s="2">
+      <c r="QI1" s="1">
         <v>44377</v>
       </c>
-      <c r="QJ1" s="2">
+      <c r="QJ1" s="1">
         <v>44378</v>
       </c>
-      <c r="QK1" s="2">
+      <c r="QK1" s="1">
         <v>44379</v>
       </c>
-      <c r="QL1" s="2">
+      <c r="QL1" s="1">
         <v>44380</v>
       </c>
-      <c r="QM1" s="2">
+      <c r="QM1" s="1">
         <v>44381</v>
       </c>
-      <c r="QN1" s="2">
+      <c r="QN1" s="1">
         <v>44382</v>
       </c>
-      <c r="QO1" s="2">
+      <c r="QO1" s="1">
         <v>44383</v>
       </c>
-      <c r="QP1" s="2">
+      <c r="QP1" s="1">
         <v>44384</v>
       </c>
-      <c r="QQ1" s="2">
+      <c r="QQ1" s="1">
         <v>44385</v>
       </c>
-      <c r="QR1" s="2">
+      <c r="QR1" s="1">
         <v>44386</v>
       </c>
-      <c r="QS1" s="2">
+      <c r="QS1" s="1">
         <v>44387</v>
       </c>
-      <c r="QT1" s="2">
+      <c r="QT1" s="1">
         <v>44388</v>
       </c>
-      <c r="QU1" s="2">
+      <c r="QU1" s="1">
         <v>44389</v>
       </c>
-      <c r="QV1" s="2">
+      <c r="QV1" s="1">
         <v>44390</v>
       </c>
-      <c r="QW1" s="2">
+      <c r="QW1" s="1">
         <v>44391</v>
       </c>
-      <c r="QX1" s="2">
+      <c r="QX1" s="1">
         <v>44392</v>
       </c>
-      <c r="QY1" s="2">
+      <c r="QY1" s="1">
         <v>44393</v>
       </c>
-      <c r="QZ1" s="2">
+      <c r="QZ1" s="1">
         <v>44394</v>
       </c>
-      <c r="RA1" s="2">
+      <c r="RA1" s="1">
         <v>44395</v>
       </c>
-      <c r="RB1" s="2">
+      <c r="RB1" s="1">
         <v>44396</v>
       </c>
-      <c r="RC1" s="2">
+      <c r="RC1" s="1">
         <v>44397</v>
       </c>
-      <c r="RD1" s="2">
+      <c r="RD1" s="1">
         <v>44398</v>
       </c>
-      <c r="RE1" s="2">
+      <c r="RE1" s="1">
         <v>44399</v>
       </c>
+      <c r="RF1" s="1">
+        <v>44400</v>
+      </c>
+      <c r="RG1" s="1">
+        <v>44401</v>
+      </c>
+      <c r="RH1" s="1">
+        <v>44402</v>
+      </c>
+      <c r="RI1" s="1">
+        <v>44403</v>
+      </c>
+      <c r="RJ1" s="1">
+        <v>44404</v>
+      </c>
+      <c r="RK1" s="1">
+        <v>44405</v>
+      </c>
+      <c r="RL1" s="1">
+        <v>44406</v>
+      </c>
+      <c r="RM1" s="1">
+        <v>44407</v>
+      </c>
+      <c r="RN1" s="1">
+        <v>44408</v>
+      </c>
+      <c r="RO1" s="1">
+        <v>44409</v>
+      </c>
+      <c r="RP1" s="1">
+        <v>44410</v>
+      </c>
+      <c r="RQ1" s="1">
+        <v>44411</v>
+      </c>
+      <c r="RR1" s="1">
+        <v>44412</v>
+      </c>
+      <c r="RS1" s="1">
+        <v>44413</v>
+      </c>
+      <c r="RT1" s="1">
+        <v>44414</v>
+      </c>
+      <c r="RU1" s="1">
+        <v>44415</v>
+      </c>
+      <c r="RV1" s="1">
+        <v>44416</v>
+      </c>
+      <c r="RW1" s="1">
+        <v>44417</v>
+      </c>
+      <c r="RX1" s="1">
+        <v>44418</v>
+      </c>
+      <c r="RY1" s="1">
+        <v>44419</v>
+      </c>
+      <c r="RZ1" s="1">
+        <v>44420</v>
+      </c>
     </row>
-    <row r="2" spans="1:473" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:494" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>34.142857142857146</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>31.571428571428573</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>29.428571428571427</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>28</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>26</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>24.857142857142858</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>23.714285714285715</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>23.285714285714285</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>23.285714285714285</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>23</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>23.714285714285715</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>24.428571428571427</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
         <v>25.285714285714285</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>26.571428571428573</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>28.142857142857142</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="Q2" s="4">
         <v>28.428571428571427</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="4">
         <v>28.857142857142858</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="4">
         <v>28.857142857142858</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <v>29.142857142857142</v>
       </c>
-      <c r="U2" s="5">
+      <c r="U2" s="4">
         <v>29.571428571428573</v>
       </c>
-      <c r="V2" s="5">
+      <c r="V2" s="4">
         <v>30.142857142857142</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="4">
         <v>29.428571428571427</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="4">
         <v>30.714285714285715</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Y2" s="4">
         <v>31.571428571428573</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="4">
         <v>34.714285714285715</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2" s="4">
         <v>36.142857142857146</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="AB2" s="4">
         <v>38.714285714285715</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="AC2" s="4">
         <v>40.714285714285715</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AD2" s="4">
         <v>45.571428571428569</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AE2" s="4">
         <v>49.571428571428569</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AF2" s="4">
         <v>54.142857142857146</v>
       </c>
-      <c r="AG2" s="5">
+      <c r="AG2" s="4">
         <v>56.285714285714285</v>
       </c>
-      <c r="AH2" s="5">
+      <c r="AH2" s="4">
         <v>59.428571428571431</v>
       </c>
-      <c r="AI2" s="5">
+      <c r="AI2" s="4">
         <v>61.857142857142854</v>
       </c>
-      <c r="AJ2" s="5">
+      <c r="AJ2" s="4">
         <v>67.714285714285708</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AK2" s="4">
         <v>69.142857142857139</v>
       </c>
-      <c r="AL2" s="5">
+      <c r="AL2" s="4">
         <v>75.571428571428569</v>
       </c>
-      <c r="AM2" s="5">
+      <c r="AM2" s="4">
         <v>79</v>
       </c>
-      <c r="AN2" s="5">
+      <c r="AN2" s="4">
         <v>83.571428571428569</v>
       </c>
-      <c r="AO2" s="5">
+      <c r="AO2" s="4">
         <v>93.714285714285708</v>
       </c>
-      <c r="AP2" s="5">
+      <c r="AP2" s="4">
         <v>100.28571428571429</v>
       </c>
-      <c r="AQ2" s="5">
+      <c r="AQ2" s="4">
         <v>104.57142857142857</v>
       </c>
-      <c r="AR2" s="5">
+      <c r="AR2" s="4">
         <v>112.57142857142857</v>
       </c>
-      <c r="AS2" s="5">
+      <c r="AS2" s="4">
         <v>118.85714285714286</v>
       </c>
-      <c r="AT2" s="5">
+      <c r="AT2" s="4">
         <v>123.14285714285714</v>
       </c>
-      <c r="AU2" s="5">
+      <c r="AU2" s="4">
         <v>125.85714285714286</v>
       </c>
-      <c r="AV2" s="5">
+      <c r="AV2" s="4">
         <v>125.28571428571429</v>
       </c>
-      <c r="AW2" s="5">
+      <c r="AW2" s="4">
         <v>127</v>
       </c>
-      <c r="AX2" s="5">
+      <c r="AX2" s="4">
         <v>130.57142857142858</v>
       </c>
-      <c r="AY2" s="5">
+      <c r="AY2" s="4">
         <v>135.42857142857142</v>
       </c>
-      <c r="AZ2" s="5">
+      <c r="AZ2" s="4">
         <v>135.28571428571428</v>
       </c>
-      <c r="BA2" s="5">
+      <c r="BA2" s="4">
         <v>136.14285714285714</v>
       </c>
-      <c r="BB2" s="5">
+      <c r="BB2" s="4">
         <v>139.28571428571428</v>
       </c>
-      <c r="BC2" s="5">
+      <c r="BC2" s="4">
         <v>142.28571428571428</v>
       </c>
-      <c r="BD2" s="5">
+      <c r="BD2" s="4">
         <v>141.42857142857142</v>
       </c>
-      <c r="BE2" s="5">
+      <c r="BE2" s="4">
         <v>141.42857142857142</v>
       </c>
-      <c r="BF2" s="5">
+      <c r="BF2" s="4">
         <v>138</v>
       </c>
-      <c r="BG2" s="5">
+      <c r="BG2" s="4">
         <v>140</v>
       </c>
-      <c r="BH2" s="5">
+      <c r="BH2" s="4">
         <v>142.57142857142858</v>
       </c>
-      <c r="BI2" s="5">
+      <c r="BI2" s="4">
         <v>143.14285714285714</v>
       </c>
-      <c r="BJ2" s="5">
+      <c r="BJ2" s="4">
         <v>143</v>
       </c>
-      <c r="BK2" s="5">
+      <c r="BK2" s="4">
         <v>144.28571428571428</v>
       </c>
-      <c r="BL2" s="5">
+      <c r="BL2" s="4">
         <v>142</v>
       </c>
-      <c r="BM2" s="5">
+      <c r="BM2" s="4">
         <v>142.71428571428572</v>
       </c>
-      <c r="BN2" s="5">
+      <c r="BN2" s="4">
         <v>141.14285714285714</v>
       </c>
-      <c r="BO2" s="5">
+      <c r="BO2" s="4">
         <v>138.14285714285714</v>
       </c>
-      <c r="BP2" s="5">
+      <c r="BP2" s="4">
         <v>140</v>
       </c>
-      <c r="BQ2" s="5">
+      <c r="BQ2" s="4">
         <v>139.85714285714286</v>
       </c>
-      <c r="BR2" s="5">
+      <c r="BR2" s="4">
         <v>139.57142857142858</v>
       </c>
-      <c r="BS2" s="5">
+      <c r="BS2" s="4">
         <v>141.85714285714286</v>
       </c>
-      <c r="BT2" s="5">
+      <c r="BT2" s="4">
         <v>141.14285714285714</v>
       </c>
-      <c r="BU2" s="5">
+      <c r="BU2" s="4">
         <v>138.57142857142858</v>
       </c>
-      <c r="BV2" s="5">
+      <c r="BV2" s="4">
         <v>140.28571428571428</v>
       </c>
-      <c r="BW2" s="5">
+      <c r="BW2" s="4">
         <v>137.85714285714286</v>
       </c>
-      <c r="BX2" s="5">
+      <c r="BX2" s="4">
         <v>133.57142857142858</v>
       </c>
-      <c r="BY2" s="5">
+      <c r="BY2" s="4">
         <v>130.85714285714286</v>
       </c>
-      <c r="BZ2" s="5">
+      <c r="BZ2" s="4">
         <v>130.28571428571428</v>
       </c>
-      <c r="CA2" s="5">
+      <c r="CA2" s="4">
         <v>124.42857142857143</v>
       </c>
-      <c r="CB2" s="5">
+      <c r="CB2" s="4">
         <v>127.14285714285714</v>
       </c>
-      <c r="CC2" s="5">
+      <c r="CC2" s="4">
         <v>125.71428571428571</v>
       </c>
-      <c r="CD2" s="5">
+      <c r="CD2" s="4">
         <v>124</v>
       </c>
-      <c r="CE2" s="5">
+      <c r="CE2" s="4">
         <v>123.14285714285714</v>
       </c>
-      <c r="CF2" s="5">
+      <c r="CF2" s="4">
         <v>124.14285714285714</v>
       </c>
-      <c r="CG2" s="5">
+      <c r="CG2" s="4">
         <v>118.14285714285714</v>
       </c>
-      <c r="CH2" s="5">
+      <c r="CH2" s="4">
         <v>119.14285714285714</v>
       </c>
-      <c r="CI2" s="5">
+      <c r="CI2" s="4">
         <v>115.85714285714286</v>
       </c>
-      <c r="CJ2" s="5">
+      <c r="CJ2" s="4">
         <v>110.85714285714286</v>
       </c>
-      <c r="CK2" s="5">
+      <c r="CK2" s="4">
         <v>109.28571428571429</v>
       </c>
-      <c r="CL2" s="5">
+      <c r="CL2" s="4">
         <v>104.42857142857143</v>
       </c>
-      <c r="CM2" s="5">
+      <c r="CM2" s="4">
         <v>102.14285714285714</v>
       </c>
-      <c r="CN2" s="5">
+      <c r="CN2" s="4">
         <v>100.71428571428571</v>
       </c>
-      <c r="CO2" s="5">
+      <c r="CO2" s="4">
         <v>99.428571428571431</v>
       </c>
-      <c r="CP2" s="5">
+      <c r="CP2" s="4">
         <v>94</v>
       </c>
-      <c r="CQ2" s="5">
+      <c r="CQ2" s="4">
         <v>93.428571428571431</v>
       </c>
-      <c r="CR2" s="5">
+      <c r="CR2" s="4">
         <v>92</v>
       </c>
-      <c r="CS2" s="5">
+      <c r="CS2" s="4">
         <v>94.571428571428569</v>
       </c>
-      <c r="CT2" s="5">
+      <c r="CT2" s="4">
         <v>89.571428571428569</v>
       </c>
-      <c r="CU2" s="5">
+      <c r="CU2" s="4">
         <v>87.571428571428569</v>
       </c>
-      <c r="CV2" s="5">
+      <c r="CV2" s="4">
         <v>84.142857142857139</v>
       </c>
-      <c r="CW2" s="5">
+      <c r="CW2" s="4">
         <v>82.571428571428569</v>
       </c>
-      <c r="CX2" s="5">
+      <c r="CX2" s="4">
         <v>78.571428571428569</v>
       </c>
-      <c r="CY2" s="5">
+      <c r="CY2" s="4">
         <v>73.571428571428569</v>
       </c>
-      <c r="CZ2" s="5">
+      <c r="CZ2" s="4">
         <v>73.285714285714292</v>
       </c>
-      <c r="DA2" s="5">
+      <c r="DA2" s="4">
         <v>73</v>
       </c>
-      <c r="DB2" s="5">
+      <c r="DB2" s="4">
         <v>72.142857142857139</v>
       </c>
-      <c r="DC2" s="5">
+      <c r="DC2" s="4">
         <v>70.714285714285708</v>
       </c>
-      <c r="DD2" s="5">
+      <c r="DD2" s="4">
         <v>69.285714285714292</v>
       </c>
-      <c r="DE2" s="5">
+      <c r="DE2" s="4">
         <v>67.428571428571431</v>
       </c>
-      <c r="DF2" s="5">
+      <c r="DF2" s="4">
         <v>67.714285714285708</v>
       </c>
-      <c r="DG2" s="5">
+      <c r="DG2" s="4">
         <v>61.142857142857146</v>
       </c>
-      <c r="DH2" s="5">
+      <c r="DH2" s="4">
         <v>59.714285714285715</v>
       </c>
-      <c r="DI2" s="5">
+      <c r="DI2" s="4">
         <v>58.285714285714285</v>
       </c>
-      <c r="DJ2" s="5">
+      <c r="DJ2" s="4">
         <v>58.857142857142854</v>
       </c>
-      <c r="DK2" s="5">
+      <c r="DK2" s="4">
         <v>57.714285714285715</v>
       </c>
-      <c r="DL2" s="5">
+      <c r="DL2" s="4">
         <v>61.285714285714285</v>
       </c>
-      <c r="DM2" s="5">
+      <c r="DM2" s="4">
         <v>57.571428571428569</v>
       </c>
-      <c r="DN2" s="5">
+      <c r="DN2" s="4">
         <v>57.857142857142854</v>
       </c>
-      <c r="DO2" s="5">
+      <c r="DO2" s="4">
         <v>56</v>
       </c>
-      <c r="DP2" s="5">
+      <c r="DP2" s="4">
         <v>54.571428571428569</v>
       </c>
-      <c r="DQ2" s="5">
+      <c r="DQ2" s="4">
         <v>52.428571428571431</v>
       </c>
-      <c r="DR2" s="5">
+      <c r="DR2" s="4">
         <v>52.714285714285715</v>
       </c>
-      <c r="DS2" s="5">
+      <c r="DS2" s="4">
         <v>50.571428571428569</v>
       </c>
-      <c r="DT2" s="5">
+      <c r="DT2" s="4">
         <v>52.285714285714285</v>
       </c>
-      <c r="DU2" s="5">
+      <c r="DU2" s="4">
         <v>53</v>
       </c>
-      <c r="DV2" s="5">
+      <c r="DV2" s="4">
         <v>52.428571428571431</v>
       </c>
-      <c r="DW2" s="5">
+      <c r="DW2" s="4">
         <v>52.142857142857146</v>
       </c>
-      <c r="DX2" s="5">
+      <c r="DX2" s="4">
         <v>50.571428571428569</v>
       </c>
-      <c r="DY2" s="5">
+      <c r="DY2" s="4">
         <v>48.857142857142854</v>
       </c>
-      <c r="DZ2" s="5">
+      <c r="DZ2" s="4">
         <v>48.285714285714285</v>
       </c>
-      <c r="EA2" s="5">
+      <c r="EA2" s="4">
         <v>46</v>
       </c>
-      <c r="EB2" s="5">
+      <c r="EB2" s="4">
         <v>44.857142857142854</v>
       </c>
-      <c r="EC2" s="5">
+      <c r="EC2" s="4">
         <v>46.285714285714285</v>
       </c>
-      <c r="ED2" s="5">
+      <c r="ED2" s="4">
         <v>45.571428571428569</v>
       </c>
-      <c r="EE2" s="5">
+      <c r="EE2" s="4">
         <v>45.714285714285715</v>
       </c>
-      <c r="EF2" s="5">
+      <c r="EF2" s="4">
         <v>47.285714285714285</v>
       </c>
-      <c r="EG2" s="5">
+      <c r="EG2" s="4">
         <v>47.285714285714285</v>
       </c>
-      <c r="EH2" s="5">
+      <c r="EH2" s="4">
         <v>48</v>
       </c>
-      <c r="EI2" s="5">
+      <c r="EI2" s="4">
         <v>48</v>
       </c>
-      <c r="EJ2" s="5">
+      <c r="EJ2" s="4">
         <v>48.285714285714285</v>
       </c>
-      <c r="EK2" s="5">
+      <c r="EK2" s="4">
         <v>48.428571428571431</v>
       </c>
-      <c r="EL2" s="5">
+      <c r="EL2" s="4">
         <v>49.285714285714285</v>
       </c>
-      <c r="EM2" s="5">
+      <c r="EM2" s="4">
         <v>45.571428571428569</v>
       </c>
-      <c r="EN2" s="5">
+      <c r="EN2" s="4">
         <v>47</v>
       </c>
-      <c r="EO2" s="5">
+      <c r="EO2" s="4">
         <v>46.285714285714285</v>
       </c>
-      <c r="EP2" s="5">
+      <c r="EP2" s="4">
         <v>45.428571428571431</v>
       </c>
-      <c r="EQ2" s="5">
+      <c r="EQ2" s="4">
         <v>44.285714285714285</v>
       </c>
-      <c r="ER2" s="5">
+      <c r="ER2" s="4">
         <v>44.142857142857146</v>
       </c>
-      <c r="ES2" s="5">
+      <c r="ES2" s="4">
         <v>44.714285714285715</v>
       </c>
-      <c r="ET2" s="5">
+      <c r="ET2" s="4">
         <v>46.714285714285715</v>
       </c>
-      <c r="EU2" s="5">
+      <c r="EU2" s="4">
         <v>45.285714285714285</v>
       </c>
-      <c r="EV2" s="5">
+      <c r="EV2" s="4">
         <v>46.142857142857146</v>
       </c>
-      <c r="EW2" s="5">
+      <c r="EW2" s="4">
         <v>46.857142857142854</v>
       </c>
-      <c r="EX2" s="5">
+      <c r="EX2" s="4">
         <v>48.714285714285715</v>
       </c>
-      <c r="EY2" s="5">
+      <c r="EY2" s="4">
         <v>51.857142857142854</v>
       </c>
-      <c r="EZ2" s="5">
+      <c r="EZ2" s="4">
         <v>51</v>
       </c>
-      <c r="FA2" s="5">
+      <c r="FA2" s="4">
         <v>50.714285714285715</v>
       </c>
-      <c r="FB2" s="5">
+      <c r="FB2" s="4">
         <v>49.857142857142854</v>
       </c>
-      <c r="FC2" s="5">
+      <c r="FC2" s="4">
         <v>50.571428571428569</v>
       </c>
-      <c r="FD2" s="5">
+      <c r="FD2" s="4">
         <v>49.285714285714285</v>
       </c>
-      <c r="FE2" s="5">
+      <c r="FE2" s="4">
         <v>48.142857142857146</v>
       </c>
-      <c r="FF2" s="5">
+      <c r="FF2" s="4">
         <v>45.571428571428569</v>
       </c>
-      <c r="FG2" s="5">
+      <c r="FG2" s="4">
         <v>47.571428571428569</v>
       </c>
-      <c r="FH2" s="5">
+      <c r="FH2" s="4">
         <v>47.285714285714285</v>
       </c>
-      <c r="FI2" s="5">
+      <c r="FI2" s="4">
         <v>47.428571428571431</v>
       </c>
-      <c r="FJ2" s="5">
+      <c r="FJ2" s="4">
         <v>46.428571428571431</v>
       </c>
-      <c r="FK2" s="5">
+      <c r="FK2" s="4">
         <v>48.285714285714285</v>
       </c>
-      <c r="FL2" s="5">
+      <c r="FL2" s="4">
         <v>48.571428571428569</v>
       </c>
-      <c r="FM2" s="5">
+      <c r="FM2" s="4">
         <v>49</v>
       </c>
-      <c r="FN2" s="5">
+      <c r="FN2" s="4">
         <v>46.142857142857146</v>
       </c>
-      <c r="FO2" s="5">
+      <c r="FO2" s="4">
         <v>46.857142857142854</v>
       </c>
-      <c r="FP2" s="5">
+      <c r="FP2" s="4">
         <v>45.285714285714285</v>
       </c>
-      <c r="FQ2" s="5">
+      <c r="FQ2" s="4">
         <v>44.285714285714285</v>
       </c>
-      <c r="FR2" s="5">
+      <c r="FR2" s="4">
         <v>43.571428571428569</v>
       </c>
-      <c r="FS2" s="5">
+      <c r="FS2" s="4">
         <v>41.142857142857146</v>
       </c>
-      <c r="FT2" s="5">
+      <c r="FT2" s="4">
         <v>39.142857142857146</v>
       </c>
-      <c r="FU2" s="5">
+      <c r="FU2" s="4">
         <v>41.857142857142854</v>
       </c>
-      <c r="FV2" s="5">
+      <c r="FV2" s="4">
         <v>42.428571428571431</v>
       </c>
-      <c r="FW2" s="5">
+      <c r="FW2" s="4">
         <v>43.571428571428569</v>
       </c>
-      <c r="FX2" s="5">
+      <c r="FX2" s="4">
         <v>43.857142857142854</v>
       </c>
-      <c r="FY2" s="5">
+      <c r="FY2" s="4">
         <v>43.142857142857146</v>
       </c>
-      <c r="FZ2" s="5">
+      <c r="FZ2" s="4">
         <v>45.857142857142854</v>
       </c>
-      <c r="GA2" s="5">
+      <c r="GA2" s="4">
         <v>46.571428571428569</v>
       </c>
-      <c r="GB2" s="5">
+      <c r="GB2" s="4">
         <v>45.428571428571431</v>
       </c>
-      <c r="GC2" s="5">
+      <c r="GC2" s="4">
         <v>44.285714285714285</v>
       </c>
-      <c r="GD2" s="5">
+      <c r="GD2" s="4">
         <v>44.142857142857146</v>
       </c>
-      <c r="GE2" s="5">
+      <c r="GE2" s="4">
         <v>45.142857142857146</v>
       </c>
-      <c r="GF2" s="5">
+      <c r="GF2" s="4">
         <v>46.428571428571431</v>
       </c>
-      <c r="GG2" s="5">
+      <c r="GG2" s="4">
         <v>45.571428571428569</v>
       </c>
-      <c r="GH2" s="5">
+      <c r="GH2" s="4">
         <v>44.285714285714285</v>
       </c>
-      <c r="GI2" s="5">
+      <c r="GI2" s="4">
         <v>43</v>
       </c>
-      <c r="GJ2" s="5">
+      <c r="GJ2" s="4">
         <v>42.571428571428569</v>
       </c>
-      <c r="GK2" s="5">
+      <c r="GK2" s="4">
         <v>41.714285714285715</v>
       </c>
-      <c r="GL2" s="5">
+      <c r="GL2" s="4">
         <v>41.857142857142854</v>
       </c>
-      <c r="GM2" s="5">
+      <c r="GM2" s="4">
         <v>40.857142857142854</v>
       </c>
-      <c r="GN2" s="5">
+      <c r="GN2" s="4">
         <v>40.285714285714285</v>
       </c>
-      <c r="GO2" s="5">
+      <c r="GO2" s="4">
         <v>41.285714285714285</v>
       </c>
-      <c r="GP2" s="5">
+      <c r="GP2" s="4">
         <v>40.857142857142854</v>
       </c>
-      <c r="GQ2" s="5">
+      <c r="GQ2" s="4">
         <v>41</v>
       </c>
-      <c r="GR2" s="5">
+      <c r="GR2" s="4">
         <v>42</v>
       </c>
-      <c r="GS2" s="5">
+      <c r="GS2" s="4">
         <v>40.714285714285715</v>
       </c>
-      <c r="GT2" s="5">
+      <c r="GT2" s="4">
         <v>40.571428571428569</v>
       </c>
-      <c r="GU2" s="5">
+      <c r="GU2" s="4">
         <v>40.142857142857146</v>
       </c>
-      <c r="GV2" s="5">
+      <c r="GV2" s="4">
         <v>40.142857142857146</v>
       </c>
-      <c r="GW2" s="5">
+      <c r="GW2" s="4">
         <v>42.285714285714285</v>
       </c>
-      <c r="GX2" s="5">
+      <c r="GX2" s="4">
         <v>40.142857142857146</v>
       </c>
-      <c r="GY2" s="5">
+      <c r="GY2" s="4">
         <v>37.714285714285715</v>
       </c>
-      <c r="GZ2" s="5">
+      <c r="GZ2" s="4">
         <v>37.571428571428569</v>
       </c>
-      <c r="HA2" s="5">
+      <c r="HA2" s="4">
         <v>37.428571428571431</v>
       </c>
-      <c r="HB2" s="5">
+      <c r="HB2" s="4">
         <v>37.285714285714285</v>
       </c>
-      <c r="HC2" s="5">
+      <c r="HC2" s="4">
         <v>37.857142857142854</v>
       </c>
-      <c r="HD2" s="5">
+      <c r="HD2" s="4">
         <v>35.571428571428569</v>
       </c>
-      <c r="HE2" s="5">
+      <c r="HE2" s="4">
         <v>36.285714285714285</v>
       </c>
-      <c r="HF2" s="5">
+      <c r="HF2" s="4">
         <v>37.428571428571431</v>
       </c>
-      <c r="HG2" s="5">
+      <c r="HG2" s="4">
         <v>37.142857142857146</v>
       </c>
-      <c r="HH2" s="5">
+      <c r="HH2" s="4">
         <v>38</v>
       </c>
-      <c r="HI2" s="5">
+      <c r="HI2" s="4">
         <v>38.428571428571431</v>
       </c>
-      <c r="HJ2" s="5">
+      <c r="HJ2" s="4">
         <v>36.285714285714285</v>
       </c>
-      <c r="HK2" s="5">
+      <c r="HK2" s="4">
         <v>36.142857142857146</v>
       </c>
-      <c r="HL2" s="5">
+      <c r="HL2" s="4">
         <v>37.428571428571431</v>
       </c>
-      <c r="HM2" s="5">
+      <c r="HM2" s="4">
         <v>36.714285714285715</v>
       </c>
-      <c r="HN2" s="5">
+      <c r="HN2" s="4">
         <v>36</v>
       </c>
-      <c r="HO2" s="5">
+      <c r="HO2" s="4">
         <v>34.714285714285715</v>
       </c>
-      <c r="HP2" s="5">
+      <c r="HP2" s="4">
         <v>34.428571428571431</v>
       </c>
-      <c r="HQ2" s="5">
+      <c r="HQ2" s="4">
         <v>36.714285714285715</v>
       </c>
-      <c r="HR2" s="5">
+      <c r="HR2" s="4">
         <v>36.428571428571431</v>
       </c>
-      <c r="HS2" s="5">
+      <c r="HS2" s="4">
         <v>37.285714285714285</v>
       </c>
-      <c r="HT2" s="5">
+      <c r="HT2" s="4">
         <v>37.714285714285715</v>
       </c>
-      <c r="HU2" s="5">
+      <c r="HU2" s="4">
         <v>38.142857142857146</v>
       </c>
-      <c r="HV2" s="5">
+      <c r="HV2" s="4">
         <v>38.571428571428569</v>
       </c>
-      <c r="HW2" s="5">
+      <c r="HW2" s="4">
         <v>37.857142857142854</v>
       </c>
-      <c r="HX2" s="5">
+      <c r="HX2" s="4">
         <v>37.857142857142854</v>
       </c>
-      <c r="HY2" s="5">
+      <c r="HY2" s="4">
         <v>36.714285714285715</v>
       </c>
-      <c r="HZ2" s="5">
+      <c r="HZ2" s="4">
         <v>35.142857142857146</v>
       </c>
-      <c r="IA2" s="5">
+      <c r="IA2" s="4">
         <v>36</v>
       </c>
-      <c r="IB2" s="5">
+      <c r="IB2" s="4">
         <v>37</v>
       </c>
-      <c r="IC2" s="5">
+      <c r="IC2" s="4">
         <v>36.714285714285715</v>
       </c>
-      <c r="ID2" s="5">
+      <c r="ID2" s="4">
         <v>37.857142857142854</v>
       </c>
-      <c r="IE2" s="5">
+      <c r="IE2" s="4">
         <v>35.857142857142854</v>
       </c>
-      <c r="IF2" s="5">
+      <c r="IF2" s="4">
         <v>37.142857142857146</v>
       </c>
-      <c r="IG2" s="5">
+      <c r="IG2" s="4">
         <v>35.714285714285715</v>
       </c>
-      <c r="IH2" s="5">
+      <c r="IH2" s="4">
         <v>35.428571428571431</v>
       </c>
-      <c r="II2" s="5">
+      <c r="II2" s="4">
         <v>34.857142857142854</v>
       </c>
-      <c r="IJ2" s="5">
+      <c r="IJ2" s="4">
         <v>34.142857142857146</v>
       </c>
-      <c r="IK2" s="5">
+      <c r="IK2" s="4">
         <v>33.714285714285715</v>
       </c>
-      <c r="IL2" s="5">
+      <c r="IL2" s="4">
         <v>35.428571428571431</v>
       </c>
-      <c r="IM2" s="5">
+      <c r="IM2" s="4">
         <v>34</v>
       </c>
-      <c r="IN2" s="5">
+      <c r="IN2" s="4">
         <v>35.428571428571431</v>
       </c>
-      <c r="IO2" s="5">
+      <c r="IO2" s="4">
         <v>36</v>
       </c>
-      <c r="IP2" s="5">
+      <c r="IP2" s="4">
         <v>36.285714285714285</v>
       </c>
-      <c r="IQ2" s="5">
+      <c r="IQ2" s="4">
         <v>37.142857142857146</v>
       </c>
-      <c r="IR2" s="5">
+      <c r="IR2" s="4">
         <v>36</v>
       </c>
-      <c r="IS2" s="5">
+      <c r="IS2" s="4">
         <v>37.571428571428569</v>
       </c>
-      <c r="IT2" s="5">
+      <c r="IT2" s="4">
         <v>39.571428571428569</v>
       </c>
-      <c r="IU2" s="5">
+      <c r="IU2" s="4">
         <v>40.571428571428569</v>
       </c>
-      <c r="IV2" s="5">
+      <c r="IV2" s="4">
         <v>41.285714285714285</v>
       </c>
-      <c r="IW2" s="5">
+      <c r="IW2" s="4">
         <v>41.714285714285715</v>
       </c>
-      <c r="IX2" s="5">
+      <c r="IX2" s="4">
         <v>45.142857142857146</v>
       </c>
-      <c r="IY2" s="5">
+      <c r="IY2" s="4">
         <v>48</v>
       </c>
-      <c r="IZ2" s="5">
+      <c r="IZ2" s="4">
         <v>45.142857142857146</v>
       </c>
-      <c r="JA2" s="5">
+      <c r="JA2" s="4">
         <v>47.857142857142854</v>
       </c>
-      <c r="JB2" s="5">
+      <c r="JB2" s="4">
         <v>50.285714285714285</v>
       </c>
-      <c r="JC2" s="5">
+      <c r="JC2" s="4">
         <v>51.714285714285715</v>
       </c>
-      <c r="JD2" s="5">
+      <c r="JD2" s="4">
         <v>52.428571428571431</v>
       </c>
-      <c r="JE2" s="5">
+      <c r="JE2" s="4">
         <v>50.285714285714285</v>
       </c>
-      <c r="JF2" s="5">
+      <c r="JF2" s="4">
         <v>50.571428571428569</v>
       </c>
-      <c r="JG2" s="5">
+      <c r="JG2" s="4">
         <v>55</v>
       </c>
-      <c r="JH2" s="5">
+      <c r="JH2" s="4">
         <v>54</v>
       </c>
-      <c r="JI2" s="5">
+      <c r="JI2" s="4">
         <v>52</v>
       </c>
-      <c r="JJ2" s="5">
+      <c r="JJ2" s="4">
         <v>50.142857142857146</v>
       </c>
-      <c r="JK2" s="5">
+      <c r="JK2" s="4">
         <v>49.714285714285715</v>
       </c>
-      <c r="JL2" s="5">
+      <c r="JL2" s="4">
         <v>52.428571428571431</v>
       </c>
-      <c r="JM2" s="5">
+      <c r="JM2" s="4">
         <v>54.142857142857146</v>
       </c>
-      <c r="JN2" s="5">
+      <c r="JN2" s="4">
         <v>54.428571428571431</v>
       </c>
-      <c r="JO2" s="5">
+      <c r="JO2" s="4">
         <v>58.714285714285715</v>
       </c>
-      <c r="JP2" s="5">
+      <c r="JP2" s="4">
         <v>62.285714285714285</v>
       </c>
-      <c r="JQ2" s="5">
+      <c r="JQ2" s="4">
         <v>68.285714285714292</v>
       </c>
-      <c r="JR2" s="5">
+      <c r="JR2" s="4">
         <v>73.285714285714292</v>
       </c>
-      <c r="JS2" s="5">
+      <c r="JS2" s="4">
         <v>76.428571428571431</v>
       </c>
-      <c r="JT2" s="5">
+      <c r="JT2" s="4">
         <v>77.857142857142861</v>
       </c>
-      <c r="JU2" s="5">
+      <c r="JU2" s="4">
         <v>79.857142857142861</v>
       </c>
-      <c r="JV2" s="5">
+      <c r="JV2" s="4">
         <v>79.285714285714292</v>
       </c>
-      <c r="JW2" s="5">
+      <c r="JW2" s="4">
         <v>84</v>
       </c>
-      <c r="JX2" s="5">
+      <c r="JX2" s="4">
         <v>83.428571428571431</v>
       </c>
-      <c r="JY2" s="5">
+      <c r="JY2" s="4">
         <v>84.285714285714292</v>
       </c>
-      <c r="JZ2" s="5">
+      <c r="JZ2" s="4">
         <v>84</v>
       </c>
-      <c r="KA2" s="5">
+      <c r="KA2" s="4">
         <v>86.714285714285708</v>
       </c>
-      <c r="KB2" s="5">
+      <c r="KB2" s="4">
         <v>92.428571428571431</v>
       </c>
-      <c r="KC2" s="5">
+      <c r="KC2" s="4">
         <v>96.285714285714292</v>
       </c>
-      <c r="KD2" s="5">
+      <c r="KD2" s="4">
         <v>97</v>
       </c>
-      <c r="KE2" s="5">
+      <c r="KE2" s="4">
         <v>98.714285714285708</v>
       </c>
-      <c r="KF2" s="5">
+      <c r="KF2" s="4">
         <v>101.85714285714286</v>
       </c>
-      <c r="KG2" s="5">
+      <c r="KG2" s="4">
         <v>102.14285714285714</v>
       </c>
-      <c r="KH2" s="5">
+      <c r="KH2" s="4">
         <v>103.28571428571429</v>
       </c>
-      <c r="KI2" s="5">
+      <c r="KI2" s="4">
         <v>103</v>
       </c>
-      <c r="KJ2" s="5">
+      <c r="KJ2" s="4">
         <v>103.85714285714286</v>
       </c>
-      <c r="KK2" s="5">
+      <c r="KK2" s="4">
         <v>105.57142857142857</v>
       </c>
-      <c r="KL2" s="5">
+      <c r="KL2" s="4">
         <v>108</v>
       </c>
-      <c r="KM2" s="5">
+      <c r="KM2" s="4">
         <v>107.85714285714286</v>
       </c>
-      <c r="KN2" s="5">
+      <c r="KN2" s="4">
         <v>110.28571428571429</v>
       </c>
-      <c r="KO2" s="5">
+      <c r="KO2" s="4">
         <v>110.71428571428571</v>
       </c>
-      <c r="KP2" s="5">
+      <c r="KP2" s="4">
         <v>110.71428571428571</v>
       </c>
-      <c r="KQ2" s="5">
+      <c r="KQ2" s="4">
         <v>111.42857142857143</v>
       </c>
-      <c r="KR2" s="5">
+      <c r="KR2" s="4">
         <v>107.42857142857143</v>
       </c>
-      <c r="KS2" s="5">
+      <c r="KS2" s="4">
         <v>105.42857142857143</v>
       </c>
-      <c r="KT2" s="5">
+      <c r="KT2" s="4">
         <v>106.28571428571429</v>
       </c>
-      <c r="KU2" s="5">
+      <c r="KU2" s="4">
         <v>106.71428571428571</v>
       </c>
-      <c r="KV2" s="5">
+      <c r="KV2" s="4">
         <v>104.42857142857143</v>
       </c>
-      <c r="KW2" s="5">
+      <c r="KW2" s="4">
         <v>101.28571428571429</v>
       </c>
-      <c r="KX2" s="5">
+      <c r="KX2" s="4">
         <v>98.571428571428569</v>
       </c>
-      <c r="KY2" s="5">
+      <c r="KY2" s="4">
         <v>100</v>
       </c>
-      <c r="KZ2" s="5">
+      <c r="KZ2" s="4">
         <v>101.28571428571429</v>
       </c>
-      <c r="LA2" s="5">
+      <c r="LA2" s="4">
         <v>102</v>
       </c>
-      <c r="LB2" s="5">
+      <c r="LB2" s="4">
         <v>100.42857142857143</v>
       </c>
-      <c r="LC2" s="5">
+      <c r="LC2" s="4">
         <v>99.142857142857139</v>
       </c>
-      <c r="LD2" s="5">
+      <c r="LD2" s="4">
         <v>98.428571428571431</v>
       </c>
-      <c r="LE2" s="5">
+      <c r="LE2" s="4">
         <v>100.71428571428571</v>
       </c>
-      <c r="LF2" s="5">
+      <c r="LF2" s="4">
         <v>101.14285714285714</v>
       </c>
-      <c r="LG2" s="5">
+      <c r="LG2" s="4">
         <v>102.71428571428571</v>
       </c>
-      <c r="LH2" s="5">
+      <c r="LH2" s="4">
         <v>100.85714285714286</v>
       </c>
-      <c r="LI2" s="5">
+      <c r="LI2" s="4">
         <v>101.71428571428571</v>
       </c>
-      <c r="LJ2" s="5">
+      <c r="LJ2" s="4">
         <v>104.14285714285714</v>
       </c>
-      <c r="LK2" s="5">
+      <c r="LK2" s="4">
         <v>103</v>
       </c>
-      <c r="LL2" s="5">
+      <c r="LL2" s="4">
         <v>104.57142857142857</v>
       </c>
-      <c r="LM2" s="5">
+      <c r="LM2" s="4">
         <v>106</v>
       </c>
-      <c r="LN2" s="5">
+      <c r="LN2" s="4">
         <v>105</v>
       </c>
-      <c r="LO2" s="5">
+      <c r="LO2" s="4">
         <v>105.71428571428571</v>
       </c>
-      <c r="LP2" s="5">
+      <c r="LP2" s="4">
         <v>107</v>
       </c>
-      <c r="LQ2" s="5">
+      <c r="LQ2" s="4">
         <v>107.85714285714286</v>
       </c>
-      <c r="LR2" s="5">
+      <c r="LR2" s="4">
         <v>110.28571428571429</v>
       </c>
-      <c r="LS2" s="5">
+      <c r="LS2" s="4">
         <v>109.42857142857143</v>
       </c>
-      <c r="LT2" s="5">
+      <c r="LT2" s="4">
         <v>110.71428571428571</v>
       </c>
-      <c r="LU2" s="5">
+      <c r="LU2" s="4">
         <v>116.28571428571429</v>
       </c>
-      <c r="LV2" s="5">
+      <c r="LV2" s="4">
         <v>122.14285714285714</v>
       </c>
-      <c r="LW2" s="5">
+      <c r="LW2" s="4">
         <v>126.14285714285714</v>
       </c>
-      <c r="LX2" s="5">
+      <c r="LX2" s="4">
         <v>131.14285714285714</v>
       </c>
-      <c r="LY2" s="5">
+      <c r="LY2" s="4">
         <v>134.42857142857142</v>
       </c>
-      <c r="LZ2" s="5">
+      <c r="LZ2" s="4">
         <v>139.57142857142858</v>
       </c>
-      <c r="MA2" s="5">
+      <c r="MA2" s="4">
         <v>142.85714285714286</v>
       </c>
-      <c r="MB2" s="5">
+      <c r="MB2" s="4">
         <v>142.71428571428572</v>
       </c>
-      <c r="MC2" s="5">
+      <c r="MC2" s="4">
         <v>143.85714285714286</v>
       </c>
-      <c r="MD2" s="5">
+      <c r="MD2" s="4">
         <v>145.28571428571428</v>
       </c>
-      <c r="ME2" s="5">
+      <c r="ME2" s="4">
         <v>148.14285714285714</v>
       </c>
-      <c r="MF2" s="5">
+      <c r="MF2" s="4">
         <v>152.85714285714286</v>
       </c>
-      <c r="MG2" s="5">
+      <c r="MG2" s="4">
         <v>156.14285714285714</v>
       </c>
-      <c r="MH2" s="5">
+      <c r="MH2" s="4">
         <v>158.85714285714286</v>
       </c>
-      <c r="MI2" s="5">
+      <c r="MI2" s="4">
         <v>166</v>
       </c>
-      <c r="MJ2" s="5">
+      <c r="MJ2" s="4">
         <v>166.71428571428572</v>
       </c>
-      <c r="MK2" s="5">
+      <c r="MK2" s="4">
         <v>172.14285714285714</v>
       </c>
-      <c r="ML2" s="5">
+      <c r="ML2" s="4">
         <v>173</v>
       </c>
-      <c r="MM2" s="5">
+      <c r="MM2" s="4">
         <v>177.71428571428572</v>
       </c>
-      <c r="MN2" s="5">
+      <c r="MN2" s="4">
         <v>179.57142857142858</v>
       </c>
-      <c r="MO2" s="5">
+      <c r="MO2" s="4">
         <v>183.85714285714286</v>
       </c>
-      <c r="MP2" s="5">
+      <c r="MP2" s="4">
         <v>188.85714285714286</v>
       </c>
-      <c r="MQ2" s="5">
+      <c r="MQ2" s="4">
         <v>190.14285714285714</v>
       </c>
-      <c r="MR2" s="5">
+      <c r="MR2" s="4">
         <v>189.85714285714286</v>
       </c>
-      <c r="MS2" s="5">
+      <c r="MS2" s="4">
         <v>197.14285714285714</v>
       </c>
-      <c r="MT2" s="5">
+      <c r="MT2" s="4">
         <v>201</v>
       </c>
-      <c r="MU2" s="5">
+      <c r="MU2" s="4">
         <v>207.42857142857142</v>
       </c>
-      <c r="MV2" s="5">
+      <c r="MV2" s="4">
         <v>210.42857142857142</v>
       </c>
-      <c r="MW2" s="5">
+      <c r="MW2" s="4">
         <v>208.42857142857142</v>
       </c>
-      <c r="MX2" s="5">
+      <c r="MX2" s="4">
         <v>214</v>
       </c>
-      <c r="MY2" s="5">
+      <c r="MY2" s="4">
         <v>217.14285714285714</v>
       </c>
-      <c r="MZ2" s="5">
+      <c r="MZ2" s="4">
         <v>216.71428571428572</v>
       </c>
-      <c r="NA2" s="5">
+      <c r="NA2" s="4">
         <v>221.28571428571428</v>
       </c>
-      <c r="NB2" s="5">
+      <c r="NB2" s="4">
         <v>224.42857142857142</v>
       </c>
-      <c r="NC2" s="5">
+      <c r="NC2" s="4">
         <v>227.71428571428572</v>
       </c>
-      <c r="ND2" s="5">
+      <c r="ND2" s="4">
         <v>232.28571428571428</v>
       </c>
-      <c r="NE2" s="5">
+      <c r="NE2" s="4">
         <v>236.85714285714286</v>
       </c>
-      <c r="NF2" s="5">
+      <c r="NF2" s="4">
         <v>237.42857142857142</v>
       </c>
-      <c r="NG2" s="5">
+      <c r="NG2" s="4">
         <v>236.57142857142858</v>
       </c>
-      <c r="NH2" s="5">
+      <c r="NH2" s="4">
         <v>231.57142857142858</v>
       </c>
-      <c r="NI2" s="5">
+      <c r="NI2" s="4">
         <v>223.85714285714286</v>
       </c>
-      <c r="NJ2" s="5">
+      <c r="NJ2" s="4">
         <v>226</v>
       </c>
-      <c r="NK2" s="5">
+      <c r="NK2" s="4">
         <v>222.14285714285714</v>
       </c>
-      <c r="NL2" s="5">
+      <c r="NL2" s="4">
         <v>219.85714285714286</v>
       </c>
-      <c r="NM2" s="5">
+      <c r="NM2" s="4">
         <v>219.14285714285714</v>
       </c>
-      <c r="NN2" s="5">
+      <c r="NN2" s="4">
         <v>217</v>
       </c>
-      <c r="NO2" s="5">
+      <c r="NO2" s="4">
         <v>216.42857142857142</v>
       </c>
-      <c r="NP2" s="5">
+      <c r="NP2" s="4">
         <v>219.57142857142858</v>
       </c>
-      <c r="NQ2" s="5">
+      <c r="NQ2" s="4">
         <v>217.42857142857142</v>
       </c>
-      <c r="NR2" s="5">
+      <c r="NR2" s="4">
         <v>213.28571428571428</v>
       </c>
-      <c r="NS2" s="5">
+      <c r="NS2" s="4">
         <v>207.71428571428572</v>
       </c>
-      <c r="NT2" s="5">
+      <c r="NT2" s="4">
         <v>201</v>
       </c>
-      <c r="NU2" s="5">
+      <c r="NU2" s="4">
         <v>201.57142857142858</v>
       </c>
-      <c r="NV2" s="5">
+      <c r="NV2" s="4">
         <v>200.71428571428572</v>
       </c>
-      <c r="NW2" s="5">
+      <c r="NW2" s="4">
         <v>195.85714285714286</v>
       </c>
-      <c r="NX2" s="5">
+      <c r="NX2" s="4">
         <v>191.14285714285714</v>
       </c>
-      <c r="NY2" s="5">
+      <c r="NY2" s="4">
         <v>193.28571428571428</v>
       </c>
-      <c r="NZ2" s="5">
+      <c r="NZ2" s="4">
         <v>194</v>
       </c>
-      <c r="OA2" s="5">
+      <c r="OA2" s="4">
         <v>192.71428571428572</v>
       </c>
-      <c r="OB2" s="5">
+      <c r="OB2" s="4">
         <v>188</v>
       </c>
-      <c r="OC2" s="5">
+      <c r="OC2" s="4">
         <v>185.71428571428572</v>
       </c>
-      <c r="OD2" s="5">
+      <c r="OD2" s="4">
         <v>182.14285714285714</v>
       </c>
-      <c r="OE2" s="5">
+      <c r="OE2" s="4">
         <v>176.42857142857142</v>
       </c>
-      <c r="OF2" s="5">
+      <c r="OF2" s="4">
         <v>170.42857142857142</v>
       </c>
-      <c r="OG2" s="5">
+      <c r="OG2" s="4">
         <v>168</v>
       </c>
-      <c r="OH2" s="5">
+      <c r="OH2" s="4">
         <v>167.85714285714286</v>
       </c>
-      <c r="OI2" s="6">
+      <c r="OI2" s="5">
         <v>163.42857142857142</v>
       </c>
-      <c r="OJ2" s="5">
+      <c r="OJ2" s="4">
         <v>157.85714285714286</v>
       </c>
-      <c r="OK2" s="5">
+      <c r="OK2" s="4">
         <v>160</v>
       </c>
-      <c r="OL2" s="5">
+      <c r="OL2" s="4">
         <v>158</v>
       </c>
-      <c r="OM2" s="5">
+      <c r="OM2" s="4">
         <v>157</v>
       </c>
-      <c r="ON2" s="5">
+      <c r="ON2" s="4">
         <v>157.28571428571428</v>
       </c>
-      <c r="OO2" s="5">
+      <c r="OO2" s="4">
         <v>160.14285714285714</v>
       </c>
-      <c r="OP2" s="5">
+      <c r="OP2" s="4">
         <v>164.57142857142858</v>
       </c>
-      <c r="OQ2" s="5">
+      <c r="OQ2" s="4">
         <v>166.71428571428572</v>
       </c>
-      <c r="OR2" s="5">
+      <c r="OR2" s="4">
         <v>167.28571428571428</v>
       </c>
-      <c r="OS2" s="5">
+      <c r="OS2" s="4">
         <v>170.14285714285714</v>
       </c>
-      <c r="OT2" s="5">
+      <c r="OT2" s="4">
         <v>177.85714285714286</v>
       </c>
-      <c r="OU2" s="5">
+      <c r="OU2" s="4">
         <v>178.85714285714286</v>
       </c>
-      <c r="OV2" s="5">
+      <c r="OV2" s="4">
         <v>180.42857142857142</v>
       </c>
-      <c r="OW2" s="5">
+      <c r="OW2" s="4">
         <v>183.42857142857142</v>
       </c>
-      <c r="OX2" s="5">
+      <c r="OX2" s="4">
         <v>185.42857142857142</v>
       </c>
-      <c r="OY2" s="5">
+      <c r="OY2" s="4">
+        <v>189</v>
+      </c>
+      <c r="OZ2" s="4">
+        <v>196</v>
+      </c>
+      <c r="PA2" s="4">
+        <v>195.85714285714286</v>
+      </c>
+      <c r="PB2" s="4">
+        <v>202</v>
+      </c>
+      <c r="PC2" s="4">
+        <v>203.42857142857142</v>
+      </c>
+      <c r="PD2" s="4">
+        <v>206.85714285714286</v>
+      </c>
+      <c r="PE2" s="4">
+        <v>210.85714285714286</v>
+      </c>
+      <c r="PF2" s="4">
+        <v>209.71428571428572</v>
+      </c>
+      <c r="PG2" s="4">
+        <v>208.71428571428572</v>
+      </c>
+      <c r="PH2" s="4">
+        <v>207.57142857142858</v>
+      </c>
+      <c r="PI2" s="4">
+        <v>205</v>
+      </c>
+      <c r="PJ2" s="4">
+        <v>203.28571428571428</v>
+      </c>
+      <c r="PK2" s="4">
+        <v>201.28571428571428</v>
+      </c>
+      <c r="PL2" s="4">
+        <v>204.28571428571428</v>
+      </c>
+      <c r="PM2" s="4">
+        <v>208.28571428571428</v>
+      </c>
+      <c r="PN2" s="4">
+        <v>207.57142857142858</v>
+      </c>
+      <c r="PO2" s="4">
+        <v>205.42857142857142</v>
+      </c>
+      <c r="PP2" s="4">
+        <v>200.57142857142858</v>
+      </c>
+      <c r="PQ2" s="4">
+        <v>200.14285714285714</v>
+      </c>
+      <c r="PR2" s="4">
+        <v>203.85714285714286</v>
+      </c>
+      <c r="PS2" s="4">
+        <v>197</v>
+      </c>
+      <c r="PT2" s="4">
+        <v>194.14285714285714</v>
+      </c>
+      <c r="PU2" s="4">
         <v>188.85714285714286</v>
       </c>
-      <c r="OZ2" s="5">
-        <v>195.85714285714286</v>
-      </c>
-      <c r="PA2" s="5">
-        <v>195.71428571428572</v>
-      </c>
-      <c r="PB2" s="5">
-        <v>201.71428571428572</v>
-      </c>
-      <c r="PC2" s="5">
-        <v>203.14285714285714</v>
-      </c>
-      <c r="PD2" s="5">
-        <v>206.57142857142858</v>
-      </c>
-      <c r="PE2" s="5">
-        <v>210.57142857142858</v>
-      </c>
-      <c r="PF2" s="5">
-        <v>209.57142857142858</v>
-      </c>
-      <c r="PG2" s="5">
-        <v>208.57142857142858</v>
-      </c>
-      <c r="PH2" s="5">
-        <v>207.42857142857142</v>
-      </c>
-      <c r="PI2" s="5">
-        <v>204.85714285714286</v>
-      </c>
-      <c r="PJ2" s="5">
-        <v>203.14285714285714</v>
-      </c>
-      <c r="PK2" s="5">
-        <v>201.14285714285714</v>
-      </c>
-      <c r="PL2" s="5">
-        <v>204.14285714285714</v>
-      </c>
-      <c r="PM2" s="5">
-        <v>208.14285714285714</v>
-      </c>
-      <c r="PN2" s="5">
-        <v>207.42857142857142</v>
-      </c>
-      <c r="PO2" s="5">
-        <v>205.42857142857142</v>
-      </c>
-      <c r="PP2" s="5">
-        <v>200.71428571428572</v>
-      </c>
-      <c r="PQ2" s="5">
-        <v>200.28571428571428</v>
-      </c>
-      <c r="PR2" s="5">
-        <v>204</v>
-      </c>
-      <c r="PS2" s="5">
-        <v>197.14285714285714</v>
-      </c>
-      <c r="PT2" s="5">
-        <v>194.28571428571428</v>
-      </c>
-      <c r="PU2" s="5">
-        <v>189</v>
-      </c>
-      <c r="PV2" s="5">
+      <c r="PV2" s="4">
         <v>188.71428571428572</v>
       </c>
-      <c r="PW2" s="5">
+      <c r="PW2" s="4">
         <v>186.42857142857142</v>
       </c>
-      <c r="PX2" s="5">
+      <c r="PX2" s="4">
         <v>185.71428571428572</v>
       </c>
-      <c r="PY2" s="5">
+      <c r="PY2" s="4">
         <v>178</v>
       </c>
-      <c r="PZ2" s="5">
+      <c r="PZ2" s="4">
         <v>173.71428571428572</v>
       </c>
-      <c r="QA2" s="5">
+      <c r="QA2" s="4">
         <v>164.14285714285714</v>
       </c>
-      <c r="QB2" s="5">
+      <c r="QB2" s="4">
         <v>161.42857142857142</v>
       </c>
-      <c r="QC2" s="5">
+      <c r="QC2" s="4">
         <v>160.28571428571428</v>
       </c>
-      <c r="QD2" s="5">
+      <c r="QD2" s="4">
         <v>160.14285714285714</v>
       </c>
-      <c r="QE2" s="5">
+      <c r="QE2" s="4">
         <v>157.14285714285714</v>
       </c>
-      <c r="QF2" s="5">
+      <c r="QF2" s="4">
         <v>153</v>
       </c>
-      <c r="QG2" s="5">
+      <c r="QG2" s="4">
         <v>148.57142857142858</v>
       </c>
-      <c r="QH2" s="5">
+      <c r="QH2" s="4">
         <v>147.28571428571428</v>
       </c>
-      <c r="QI2" s="5">
+      <c r="QI2" s="4">
         <v>145.85714285714286</v>
       </c>
-      <c r="QJ2" s="5">
-        <v>137.42857142857142</v>
-      </c>
-      <c r="QK2" s="5">
-        <v>130.57142857142858</v>
-      </c>
-      <c r="QL2" s="5">
-        <v>121.85714285714286</v>
-      </c>
-      <c r="QM2" s="5">
-        <v>116.85714285714286</v>
-      </c>
-      <c r="QN2" s="5">
-        <v>113.57142857142857</v>
-      </c>
-      <c r="QO2" s="5">
-        <v>106.57142857142857</v>
-      </c>
-      <c r="QP2" s="5">
-        <v>99.571428571428569</v>
-      </c>
-      <c r="QQ2" s="5">
-        <v>93.571428571428569</v>
-      </c>
-      <c r="QR2" s="5">
-        <v>89.857142857142861</v>
-      </c>
-      <c r="QS2" s="5">
-        <v>86.571428571428569</v>
-      </c>
-      <c r="QT2" s="5">
-        <v>84.857142857142861</v>
-      </c>
-      <c r="QU2" s="5">
-        <v>82.142857142857139</v>
-      </c>
-      <c r="QV2" s="5">
-        <v>80.428571428571431</v>
-      </c>
-      <c r="QW2" s="5">
-        <v>78.285714285714292</v>
-      </c>
-      <c r="QX2" s="5">
-        <v>74.428571428571431</v>
-      </c>
-      <c r="QY2" s="5">
-        <v>69</v>
-      </c>
-      <c r="QZ2" s="5">
+      <c r="QJ2" s="4">
+        <v>137.57142857142858</v>
+      </c>
+      <c r="QK2" s="4">
+        <v>130.71428571428572</v>
+      </c>
+      <c r="QL2" s="4">
+        <v>122</v>
+      </c>
+      <c r="QM2" s="4">
+        <v>117</v>
+      </c>
+      <c r="QN2" s="4">
+        <v>113.71428571428571</v>
+      </c>
+      <c r="QO2" s="4">
+        <v>106.85714285714286</v>
+      </c>
+      <c r="QP2" s="4">
+        <v>99.857142857142861</v>
+      </c>
+      <c r="QQ2" s="4">
+        <v>93.714285714285708</v>
+      </c>
+      <c r="QR2" s="4">
+        <v>90</v>
+      </c>
+      <c r="QS2" s="4">
+        <v>87.285714285714292</v>
+      </c>
+      <c r="QT2" s="4">
+        <v>85.571428571428569</v>
+      </c>
+      <c r="QU2" s="4">
+        <v>82.857142857142861</v>
+      </c>
+      <c r="QV2" s="4">
+        <v>81</v>
+      </c>
+      <c r="QW2" s="4">
+        <v>78.857142857142861</v>
+      </c>
+      <c r="QX2" s="4">
+        <v>75</v>
+      </c>
+      <c r="QY2" s="4">
+        <v>69.571428571428569</v>
+      </c>
+      <c r="QZ2" s="4">
         <v>67.428571428571431</v>
       </c>
-      <c r="RA2" s="5">
+      <c r="RA2" s="4">
         <v>61.857142857142854</v>
       </c>
-      <c r="RB2" s="5">
+      <c r="RB2" s="4">
         <v>59.285714285714285</v>
       </c>
-      <c r="RC2" s="5">
-        <v>58</v>
-      </c>
-      <c r="RD2" s="5">
+      <c r="RC2" s="4">
+        <v>58.428571428571431</v>
+      </c>
+      <c r="RD2" s="4">
+        <v>54.857142857142854</v>
+      </c>
+      <c r="RE2" s="4">
+        <v>55.571428571428569</v>
+      </c>
+      <c r="RF2" s="6">
+        <v>56</v>
+      </c>
+      <c r="RG2" s="6">
+        <v>52.857142857142854</v>
+      </c>
+      <c r="RH2" s="6">
         <v>54</v>
       </c>
-      <c r="RE2" s="5">
-        <v>54.285714285714285</v>
+      <c r="RI2" s="6">
+        <v>51.142857142857146</v>
+      </c>
+      <c r="RJ2" s="6">
+        <v>48.142857142857146</v>
+      </c>
+      <c r="RK2" s="6">
+        <v>45.285714285714285</v>
+      </c>
+      <c r="RL2" s="6">
+        <v>43.285714285714285</v>
+      </c>
+      <c r="RM2" s="6">
+        <v>41.428571428571431</v>
+      </c>
+      <c r="RN2" s="6">
+        <v>42.285714285714285</v>
+      </c>
+      <c r="RO2" s="6">
+        <v>40.428571428571431</v>
+      </c>
+      <c r="RP2" s="6">
+        <v>41.571428571428569</v>
+      </c>
+      <c r="RQ2" s="6">
+        <v>41.571428571428569</v>
+      </c>
+      <c r="RR2" s="6">
+        <v>43.142857142857146</v>
+      </c>
+      <c r="RS2" s="6">
+        <v>41.142857142857146</v>
+      </c>
+      <c r="RT2" s="6">
+        <v>39.857142857142854</v>
+      </c>
+      <c r="RU2" s="6">
+        <v>38.285714285714285</v>
+      </c>
+      <c r="RV2" s="6">
+        <v>36.571428571428569</v>
+      </c>
+      <c r="RW2" s="6">
+        <v>35.571428571428569</v>
+      </c>
+      <c r="RX2" s="6">
+        <v>33.571428571428569</v>
+      </c>
+      <c r="RY2" s="6">
+        <v>32.571428571428569</v>
+      </c>
+      <c r="RZ2" s="6">
+        <v>33.714285714285715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>